<commit_message>
fixed some typos in rules, updated pom to 0.11
</commit_message>
<xml_diff>
--- a/src/main/resources/net/clementlevallois/umigon/heuristics/lexicons/en/en.xlsx
+++ b/src/main/resources/net/clementlevallois/umigon/heuristics/lexicons/en/en.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levallois\Google Drive\open\UmigonLambda\umigon-heuristics\src\main\java\net\clementlevallois\umigon\heuristics\resources\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levallois\open\nocode-app-functions\umigon-lexicons\src\main\resources\net\clementlevallois\umigon\heuristics\lexicons\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B049A735-6C87-46B8-9726-80CE35EEAF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F70D0C-4CAD-419A-8FE6-1FA7AC52E25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="871" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9225" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="8" r:id="rId1"/>
@@ -5270,9 +5270,6 @@
     <t>pure</t>
   </si>
   <si>
-    <t>!isImmediatelyPrecededByANegationis+++!isImmediatelyFollowedBySpecificTerm///at</t>
-  </si>
-  <si>
     <t>if (A &amp;&amp; B) {11} else {12}</t>
   </si>
   <si>
@@ -5457,6 +5454,9 @@
   </si>
   <si>
     <t>isHashtag</t>
+  </si>
+  <si>
+    <t>!isImmediatelyPrecededByANegation+++!isImmediatelyFollowedBySpecificTerm///at</t>
   </si>
 </sst>
 </file>
@@ -5498,20 +5498,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -6395,7 +6394,7 @@
         <v>365</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1457</v>
@@ -7883,7 +7882,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>328</v>
@@ -7894,7 +7893,7 @@
         <v>141</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>328</v>
@@ -7905,7 +7904,7 @@
         <v>297</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>328</v>
@@ -7938,7 +7937,7 @@
         <v>439</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>326</v>
@@ -7949,7 +7948,7 @@
         <v>440</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>326</v>
@@ -7993,7 +7992,7 @@
         <v>614</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>325</v>
@@ -8004,7 +8003,7 @@
         <v>715</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>326</v>
@@ -8015,7 +8014,7 @@
         <v>1185</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>332</v>
@@ -8026,7 +8025,7 @@
         <v>1186</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>332</v>
@@ -8037,7 +8036,7 @@
         <v>1187</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>332</v>
@@ -8048,7 +8047,7 @@
         <v>1188</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>328</v>
@@ -8059,7 +8058,7 @@
         <v>1197</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>326</v>
@@ -8070,7 +8069,7 @@
         <v>1364</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>332</v>
@@ -8081,7 +8080,7 @@
         <v>767</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>332</v>
@@ -8257,17 +8256,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
@@ -8277,22 +8276,22 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
     </row>
   </sheetData>
@@ -8304,8 +8303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E377"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8632,7 +8631,7 @@
         <v>1414</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1727</v>
@@ -8738,10 +8737,10 @@
         <v>894</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>1726</v>
@@ -8755,7 +8754,7 @@
         <v>1732</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>1726</v>
@@ -9179,7 +9178,7 @@
         <v>1498</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>1726</v>
@@ -9319,7 +9318,7 @@
         <v>1733</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>1726</v>
@@ -9333,7 +9332,7 @@
         <v>1733</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>1726</v>
@@ -9918,7 +9917,7 @@
         <v>1733</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>1726</v>
@@ -9974,7 +9973,7 @@
         <v>1735</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>1727</v>
@@ -10027,7 +10026,7 @@
         <v>46</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>1468</v>
@@ -10206,7 +10205,7 @@
         <v>1481</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>1726</v>
@@ -10248,7 +10247,7 @@
         <v>1450</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>1726</v>
@@ -10690,7 +10689,7 @@
         <v>1333</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>1726</v>
@@ -10841,7 +10840,7 @@
         <v>1449</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>1726</v>
@@ -11143,10 +11142,10 @@
         <v>1320</v>
       </c>
       <c r="B207" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C207" s="1" t="s">
         <v>1739</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>1740</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>1727</v>
@@ -11624,7 +11623,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>1469</v>
@@ -11783,7 +11782,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>1066</v>
@@ -11836,10 +11835,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>1468</v>
@@ -11912,7 +11911,7 @@
         <v>1449</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>1726</v>
@@ -12869,7 +12868,7 @@
         <v>1493</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D332" s="1" t="s">
         <v>1726</v>
@@ -13140,7 +13139,7 @@
         <v>1488</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D352" s="1" t="s">
         <v>1726</v>
@@ -13527,7 +13526,7 @@
       <c r="E3" s="2" t="s">
         <v>1726</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -13539,9 +13538,9 @@
       <c r="E4" s="2" t="s">
         <v>1726</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -14192,7 +14191,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>1082</v>
@@ -14245,7 +14244,7 @@
         <v>338</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>1082</v>
@@ -14474,7 +14473,7 @@
         <v>1061</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>1420</v>
@@ -14491,7 +14490,7 @@
         <v>1062</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>1420</v>
@@ -14740,7 +14739,7 @@
         <v>906</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>1082</v>
@@ -14821,7 +14820,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>1082</v>
@@ -15899,7 +15898,7 @@
         <v>1443</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E180" s="2" t="s">
         <v>1727</v>
@@ -16186,7 +16185,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>1082</v>
@@ -16197,7 +16196,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>1082</v>
@@ -16330,7 +16329,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>1082</v>
@@ -16341,7 +16340,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>1082</v>
@@ -16565,7 +16564,7 @@
         <v>1699</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>1082</v>
@@ -17103,7 +17102,7 @@
         <v>1206</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E275" s="2" t="s">
         <v>1727</v>
@@ -17111,7 +17110,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>1082</v>
@@ -17139,10 +17138,10 @@
         <v>755</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>1420</v>
@@ -17925,10 +17924,10 @@
         <v>963</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D338" s="2" t="s">
         <v>1420</v>
@@ -17970,7 +17969,7 @@
         <v>1445</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D341" s="2" t="s">
         <v>1420</v>
@@ -18112,7 +18111,7 @@
         <v>1515</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>1420</v>
@@ -18690,7 +18689,7 @@
         <v>1066</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E398" s="2" t="s">
         <v>1727</v>
@@ -19270,7 +19269,7 @@
         <v>1392</v>
       </c>
       <c r="C445" s="1" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D445" s="2" t="s">
         <v>1420</v>
@@ -19387,7 +19386,7 @@
         <v>1524</v>
       </c>
       <c r="C454" s="1" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="E454" s="2" t="s">
         <v>1727</v>
@@ -19426,7 +19425,7 @@
         <v>261</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C457" s="1" t="s">
         <v>1082</v>
@@ -19856,7 +19855,7 @@
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A492" s="1" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="C492" s="1" t="s">
         <v>1082</v>
@@ -19996,7 +19995,7 @@
         <v>1423</v>
       </c>
       <c r="C502" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D502" s="2" t="s">
         <v>1420</v>
@@ -20032,10 +20031,10 @@
         <v>1086</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="C505" s="5" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E505" s="2" t="s">
         <v>1726</v>
@@ -20046,10 +20045,10 @@
         <v>900</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="C506" s="5" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="E506" s="2" t="s">
         <v>1726</v>
@@ -20638,7 +20637,7 @@
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A553" s="1" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="C553" s="1" t="s">
         <v>1082</v>
@@ -20649,7 +20648,7 @@
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A554" s="1" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="C554" s="1" t="s">
         <v>1082</v>
@@ -20829,7 +20828,7 @@
         <v>1424</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="E569" s="2" t="s">
         <v>1727</v>
@@ -20843,7 +20842,7 @@
         <v>1424</v>
       </c>
       <c r="C570" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="E570" s="2" t="s">
         <v>1727</v>
@@ -21597,7 +21596,7 @@
         <v>1117</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="E634" s="2" t="s">
         <v>1726</v>
@@ -21658,7 +21657,7 @@
         <v>1529</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="E639" s="2" t="s">
         <v>1727</v>
@@ -21829,7 +21828,7 @@
         <v>1562</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="E654" s="2" t="s">
         <v>1727</v>
@@ -22628,10 +22627,10 @@
         <v>410</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D719" s="1" t="s">
         <v>1727</v>
@@ -23876,10 +23875,10 @@
         <v>248</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E818" s="2" t="s">
         <v>1726</v>
@@ -25069,691 +25068,691 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C102" s="8"/>
+      <c r="C102" s="7"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C103" s="8"/>
+      <c r="C103" s="7"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C104" s="8"/>
+      <c r="C104" s="7"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C105" s="8"/>
+      <c r="C105" s="7"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C106" s="8"/>
+      <c r="C106" s="7"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C107" s="8"/>
+      <c r="C107" s="7"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C108" s="8"/>
+      <c r="C108" s="7"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C109" s="8"/>
+      <c r="C109" s="7"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C110" s="8"/>
+      <c r="C110" s="7"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C111" s="8"/>
+      <c r="C111" s="7"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C112" s="8"/>
+      <c r="C112" s="7"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C113" s="8"/>
+      <c r="C113" s="7"/>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C114" s="8"/>
+      <c r="C114" s="7"/>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C115" s="8"/>
+      <c r="C115" s="7"/>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C116" s="8"/>
+      <c r="C116" s="7"/>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C118" s="8"/>
+      <c r="C118" s="7"/>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C119" s="8"/>
+      <c r="C119" s="7"/>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C120" s="8"/>
+      <c r="C120" s="7"/>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C122" s="8"/>
+      <c r="C122" s="7"/>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C123" s="8"/>
+      <c r="C123" s="7"/>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C124" s="8"/>
+      <c r="C124" s="7"/>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C125" s="8"/>
+      <c r="C125" s="7"/>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C126" s="8"/>
+      <c r="C126" s="7"/>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C127" s="8"/>
+      <c r="C127" s="7"/>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C128" s="8"/>
+      <c r="C128" s="7"/>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C129" s="8"/>
+      <c r="C129" s="7"/>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C130" s="8"/>
+      <c r="C130" s="7"/>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C131" s="8"/>
+      <c r="C131" s="7"/>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C134" s="8"/>
+      <c r="C134" s="7"/>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C136" s="8"/>
+      <c r="C136" s="7"/>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C137" s="8"/>
+      <c r="C137" s="7"/>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C139" s="8"/>
+      <c r="C139" s="7"/>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C140" s="8"/>
+      <c r="C140" s="7"/>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C142" s="8"/>
+      <c r="C142" s="7"/>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C143" s="8"/>
+      <c r="C143" s="7"/>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C144" s="8"/>
+      <c r="C144" s="7"/>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C145" s="8"/>
+      <c r="C145" s="7"/>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C146" s="8"/>
+      <c r="C146" s="7"/>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C147" s="8"/>
+      <c r="C147" s="7"/>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C150" s="8"/>
+      <c r="C150" s="7"/>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C152" s="8"/>
+      <c r="C152" s="7"/>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C153" s="8"/>
+      <c r="C153" s="7"/>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C154" s="8"/>
+      <c r="C154" s="7"/>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C155" s="8"/>
+      <c r="C155" s="7"/>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C156" s="8"/>
+      <c r="C156" s="7"/>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C157" s="8"/>
+      <c r="C157" s="7"/>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C159" s="8"/>
+      <c r="C159" s="7"/>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C160" s="8"/>
+      <c r="C160" s="7"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C161" s="8"/>
+      <c r="C161" s="7"/>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C162" s="8"/>
+      <c r="C162" s="7"/>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C163" s="8"/>
+      <c r="C163" s="7"/>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C164" s="8"/>
+      <c r="C164" s="7"/>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C165" s="8"/>
+      <c r="C165" s="7"/>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C166" s="8"/>
+      <c r="C166" s="7"/>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C167" s="8"/>
+      <c r="C167" s="7"/>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C168" s="8"/>
+      <c r="C168" s="7"/>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C169" s="8"/>
+      <c r="C169" s="7"/>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C170" s="8"/>
+      <c r="C170" s="7"/>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C171" s="8"/>
+      <c r="C171" s="7"/>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C172" s="8"/>
+      <c r="C172" s="7"/>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C174" s="8"/>
+      <c r="C174" s="7"/>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C175" s="8"/>
+      <c r="C175" s="7"/>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C176" s="8"/>
+      <c r="C176" s="7"/>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C178" s="8"/>
+      <c r="C178" s="7"/>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C179" s="8"/>
+      <c r="C179" s="7"/>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C180" s="8"/>
+      <c r="C180" s="7"/>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C181" s="8"/>
+      <c r="C181" s="7"/>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C182" s="8"/>
+      <c r="C182" s="7"/>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C183" s="8"/>
+      <c r="C183" s="7"/>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C185" s="8"/>
+      <c r="C185" s="7"/>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C186" s="8"/>
+      <c r="C186" s="7"/>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C187" s="8"/>
+      <c r="C187" s="7"/>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C188" s="8"/>
+      <c r="C188" s="7"/>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C189" s="8"/>
+      <c r="C189" s="7"/>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C190" s="8"/>
+      <c r="C190" s="7"/>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C191" s="8"/>
+      <c r="C191" s="7"/>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C192" s="8"/>
+      <c r="C192" s="7"/>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C193" s="8"/>
+      <c r="C193" s="7"/>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C194" s="8"/>
+      <c r="C194" s="7"/>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C196" s="8"/>
+      <c r="C196" s="7"/>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C197" s="8"/>
+      <c r="C197" s="7"/>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C198" s="8"/>
+      <c r="C198" s="7"/>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C199" s="8"/>
+      <c r="C199" s="7"/>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C200" s="8"/>
+      <c r="C200" s="7"/>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C201" s="8"/>
+      <c r="C201" s="7"/>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C202" s="8"/>
+      <c r="C202" s="7"/>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C204" s="8"/>
+      <c r="C204" s="7"/>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C205" s="8"/>
+      <c r="C205" s="7"/>
     </row>
     <row r="207" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C207" s="8"/>
+      <c r="C207" s="7"/>
     </row>
     <row r="208" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C208" s="8"/>
+      <c r="C208" s="7"/>
     </row>
     <row r="209" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C209" s="8"/>
+      <c r="C209" s="7"/>
     </row>
     <row r="210" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C210" s="8"/>
+      <c r="C210" s="7"/>
     </row>
     <row r="211" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C211" s="8"/>
+      <c r="C211" s="7"/>
     </row>
     <row r="212" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C212" s="8"/>
+      <c r="C212" s="7"/>
     </row>
     <row r="213" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C213" s="8"/>
+      <c r="C213" s="7"/>
     </row>
     <row r="214" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C214" s="8"/>
+      <c r="C214" s="7"/>
     </row>
     <row r="215" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C215" s="8"/>
+      <c r="C215" s="7"/>
     </row>
     <row r="216" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C216" s="8"/>
+      <c r="C216" s="7"/>
     </row>
     <row r="217" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C217" s="8"/>
+      <c r="C217" s="7"/>
     </row>
     <row r="218" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C218" s="8"/>
+      <c r="C218" s="7"/>
     </row>
     <row r="219" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C219" s="8"/>
+      <c r="C219" s="7"/>
     </row>
     <row r="220" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C220" s="8"/>
+      <c r="C220" s="7"/>
     </row>
     <row r="221" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C221" s="8"/>
+      <c r="C221" s="7"/>
     </row>
     <row r="222" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C222" s="8"/>
+      <c r="C222" s="7"/>
     </row>
     <row r="223" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C223" s="8"/>
+      <c r="C223" s="7"/>
     </row>
     <row r="224" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C224" s="8"/>
+      <c r="C224" s="7"/>
     </row>
     <row r="225" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C225" s="8"/>
+      <c r="C225" s="7"/>
     </row>
     <row r="226" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C226" s="8"/>
+      <c r="C226" s="7"/>
     </row>
     <row r="227" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C227" s="8"/>
+      <c r="C227" s="7"/>
     </row>
     <row r="228" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C228" s="8"/>
+      <c r="C228" s="7"/>
     </row>
     <row r="229" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C229" s="8"/>
+      <c r="C229" s="7"/>
     </row>
     <row r="230" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C230" s="8"/>
+      <c r="C230" s="7"/>
     </row>
     <row r="231" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C231" s="8"/>
+      <c r="C231" s="7"/>
     </row>
     <row r="233" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C233" s="8"/>
+      <c r="C233" s="7"/>
     </row>
     <row r="234" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C234" s="8"/>
+      <c r="C234" s="7"/>
     </row>
     <row r="235" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C235" s="8"/>
+      <c r="C235" s="7"/>
     </row>
     <row r="236" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C236" s="8"/>
+      <c r="C236" s="7"/>
     </row>
     <row r="237" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C237" s="8"/>
+      <c r="C237" s="7"/>
     </row>
     <row r="238" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C238" s="8"/>
+      <c r="C238" s="7"/>
     </row>
     <row r="239" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C239" s="8"/>
+      <c r="C239" s="7"/>
     </row>
     <row r="242" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C242" s="8"/>
+      <c r="C242" s="7"/>
     </row>
     <row r="243" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C243" s="8"/>
+      <c r="C243" s="7"/>
     </row>
     <row r="244" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C244" s="8"/>
+      <c r="C244" s="7"/>
     </row>
     <row r="245" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C245" s="8"/>
+      <c r="C245" s="7"/>
     </row>
     <row r="246" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C246" s="8"/>
+      <c r="C246" s="7"/>
     </row>
     <row r="247" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C247" s="8"/>
+      <c r="C247" s="7"/>
     </row>
     <row r="248" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C248" s="8"/>
+      <c r="C248" s="7"/>
     </row>
     <row r="251" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C251" s="8"/>
+      <c r="C251" s="7"/>
     </row>
     <row r="252" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C252" s="8"/>
+      <c r="C252" s="7"/>
     </row>
     <row r="253" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C253" s="8"/>
+      <c r="C253" s="7"/>
     </row>
     <row r="254" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C254" s="8"/>
+      <c r="C254" s="7"/>
     </row>
     <row r="256" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C256" s="8"/>
+      <c r="C256" s="7"/>
     </row>
     <row r="257" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C257" s="8"/>
+      <c r="C257" s="7"/>
     </row>
     <row r="258" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C258" s="8"/>
+      <c r="C258" s="7"/>
     </row>
     <row r="259" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C259" s="8"/>
+      <c r="C259" s="7"/>
     </row>
     <row r="260" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C260" s="8"/>
+      <c r="C260" s="7"/>
     </row>
     <row r="261" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C261" s="8"/>
+      <c r="C261" s="7"/>
     </row>
     <row r="263" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C263" s="8"/>
+      <c r="C263" s="7"/>
     </row>
     <row r="264" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C264" s="8"/>
+      <c r="C264" s="7"/>
     </row>
     <row r="265" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C265" s="8"/>
+      <c r="C265" s="7"/>
     </row>
     <row r="266" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C266" s="8"/>
+      <c r="C266" s="7"/>
     </row>
     <row r="267" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C267" s="8"/>
+      <c r="C267" s="7"/>
     </row>
     <row r="268" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C268" s="8"/>
+      <c r="C268" s="7"/>
     </row>
     <row r="270" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C270" s="8"/>
+      <c r="C270" s="7"/>
     </row>
     <row r="271" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C271" s="8"/>
+      <c r="C271" s="7"/>
     </row>
     <row r="272" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C272" s="8"/>
+      <c r="C272" s="7"/>
     </row>
     <row r="273" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C273" s="8"/>
+      <c r="C273" s="7"/>
     </row>
     <row r="274" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C274" s="8"/>
+      <c r="C274" s="7"/>
     </row>
     <row r="275" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C275" s="8"/>
+      <c r="C275" s="7"/>
     </row>
     <row r="276" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C276" s="8"/>
+      <c r="C276" s="7"/>
     </row>
     <row r="277" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C277" s="8"/>
+      <c r="C277" s="7"/>
     </row>
     <row r="278" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C278" s="8"/>
+      <c r="C278" s="7"/>
     </row>
     <row r="279" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C279" s="8"/>
+      <c r="C279" s="7"/>
     </row>
     <row r="280" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C280" s="8"/>
+      <c r="C280" s="7"/>
     </row>
     <row r="281" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C281" s="8"/>
+      <c r="C281" s="7"/>
     </row>
     <row r="282" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C282" s="8"/>
+      <c r="C282" s="7"/>
     </row>
     <row r="283" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C283" s="8"/>
+      <c r="C283" s="7"/>
     </row>
     <row r="284" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C284" s="8"/>
+      <c r="C284" s="7"/>
     </row>
     <row r="285" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C285" s="8"/>
+      <c r="C285" s="7"/>
     </row>
     <row r="286" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C286" s="8"/>
+      <c r="C286" s="7"/>
     </row>
     <row r="289" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C289" s="8"/>
+      <c r="C289" s="7"/>
     </row>
     <row r="290" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C290" s="8"/>
+      <c r="C290" s="7"/>
     </row>
     <row r="291" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C291" s="8"/>
+      <c r="C291" s="7"/>
     </row>
     <row r="293" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C293" s="8"/>
+      <c r="C293" s="7"/>
     </row>
     <row r="294" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C294" s="8"/>
+      <c r="C294" s="7"/>
     </row>
     <row r="295" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C295" s="8"/>
+      <c r="C295" s="7"/>
     </row>
     <row r="296" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C296" s="8"/>
+      <c r="C296" s="7"/>
     </row>
     <row r="297" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C297" s="8"/>
+      <c r="C297" s="7"/>
     </row>
     <row r="298" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C298" s="8"/>
+      <c r="C298" s="7"/>
     </row>
     <row r="299" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C299" s="8"/>
+      <c r="C299" s="7"/>
     </row>
     <row r="300" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C300" s="8"/>
+      <c r="C300" s="7"/>
     </row>
     <row r="301" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C301" s="8"/>
+      <c r="C301" s="7"/>
     </row>
     <row r="302" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C302" s="8"/>
+      <c r="C302" s="7"/>
     </row>
     <row r="303" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C303" s="8"/>
+      <c r="C303" s="7"/>
     </row>
     <row r="304" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C304" s="8"/>
+      <c r="C304" s="7"/>
     </row>
     <row r="305" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C305" s="8"/>
+      <c r="C305" s="7"/>
     </row>
     <row r="306" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C306" s="8"/>
+      <c r="C306" s="7"/>
     </row>
     <row r="307" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C307" s="8"/>
+      <c r="C307" s="7"/>
     </row>
     <row r="308" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C308" s="8"/>
+      <c r="C308" s="7"/>
     </row>
     <row r="309" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C309" s="8"/>
+      <c r="C309" s="7"/>
     </row>
     <row r="310" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C310" s="8"/>
+      <c r="C310" s="7"/>
     </row>
     <row r="311" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C311" s="8"/>
+      <c r="C311" s="7"/>
     </row>
     <row r="312" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C312" s="8"/>
+      <c r="C312" s="7"/>
     </row>
     <row r="313" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C313" s="8"/>
+      <c r="C313" s="7"/>
     </row>
     <row r="314" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C314" s="8"/>
+      <c r="C314" s="7"/>
     </row>
     <row r="315" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C315" s="8"/>
+      <c r="C315" s="7"/>
     </row>
     <row r="316" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C316" s="8"/>
+      <c r="C316" s="7"/>
     </row>
     <row r="317" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C317" s="8"/>
+      <c r="C317" s="7"/>
     </row>
     <row r="318" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C318" s="8"/>
+      <c r="C318" s="7"/>
     </row>
     <row r="319" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C319" s="8"/>
+      <c r="C319" s="7"/>
     </row>
     <row r="320" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C320" s="8"/>
+      <c r="C320" s="7"/>
     </row>
     <row r="321" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C321" s="8"/>
+      <c r="C321" s="7"/>
     </row>
     <row r="322" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C322" s="8"/>
+      <c r="C322" s="7"/>
     </row>
     <row r="323" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C323" s="8"/>
+      <c r="C323" s="7"/>
     </row>
     <row r="324" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C324" s="8"/>
+      <c r="C324" s="7"/>
     </row>
     <row r="325" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C325" s="8"/>
+      <c r="C325" s="7"/>
     </row>
     <row r="326" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C326" s="8"/>
+      <c r="C326" s="7"/>
     </row>
     <row r="327" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C327" s="8"/>
+      <c r="C327" s="7"/>
     </row>
     <row r="328" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C328" s="8"/>
+      <c r="C328" s="7"/>
     </row>
     <row r="329" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C329" s="8"/>
+      <c r="C329" s="7"/>
     </row>
     <row r="330" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C330" s="8"/>
+      <c r="C330" s="7"/>
     </row>
     <row r="332" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C332" s="8"/>
+      <c r="C332" s="7"/>
     </row>
     <row r="333" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C333" s="8"/>
+      <c r="C333" s="7"/>
     </row>
     <row r="334" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C334" s="8"/>
+      <c r="C334" s="7"/>
     </row>
     <row r="335" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C335" s="8"/>
+      <c r="C335" s="7"/>
     </row>
     <row r="336" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C336" s="8"/>
+      <c r="C336" s="7"/>
     </row>
     <row r="338" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C338" s="8"/>
+      <c r="C338" s="7"/>
     </row>
     <row r="339" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C339" s="8"/>
+      <c r="C339" s="7"/>
     </row>
     <row r="340" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C340" s="8"/>
+      <c r="C340" s="7"/>
     </row>
     <row r="342" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C342" s="8"/>
+      <c r="C342" s="7"/>
     </row>
     <row r="343" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C343" s="8"/>
+      <c r="C343" s="7"/>
     </row>
     <row r="344" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C344" s="8"/>
+      <c r="C344" s="7"/>
     </row>
     <row r="346" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C346" s="8"/>
+      <c r="C346" s="7"/>
     </row>
     <row r="349" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C349" s="8"/>
+      <c r="C349" s="7"/>
     </row>
     <row r="350" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C350" s="8"/>
+      <c r="C350" s="7"/>
     </row>
     <row r="354" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C354" s="8"/>
+      <c r="C354" s="7"/>
     </row>
     <row r="355" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C355" s="8"/>
+      <c r="C355" s="7"/>
     </row>
     <row r="356" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C356" s="8"/>
+      <c r="C356" s="7"/>
     </row>
     <row r="357" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C357" s="8"/>
+      <c r="C357" s="7"/>
     </row>
     <row r="359" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C359" s="8"/>
+      <c r="C359" s="7"/>
     </row>
     <row r="361" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C361" s="8"/>
+      <c r="C361" s="7"/>
     </row>
     <row r="362" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C362" s="8"/>
+      <c r="C362" s="7"/>
     </row>
     <row r="363" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C363" s="8"/>
+      <c r="C363" s="7"/>
     </row>
     <row r="366" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C366" s="8"/>
+      <c r="C366" s="7"/>
     </row>
     <row r="367" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C367" s="8"/>
+      <c r="C367" s="7"/>
     </row>
     <row r="368" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C368" s="8"/>
+      <c r="C368" s="7"/>
     </row>
     <row r="372" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C372" s="8"/>
+      <c r="C372" s="7"/>
     </row>
     <row r="375" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C375" s="8"/>
+      <c r="C375" s="7"/>
     </row>
     <row r="376" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C376" s="8"/>
+      <c r="C376" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25894,7 +25893,7 @@
         <v>708</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="C13" s="1">
         <v>22</v>
@@ -26286,7 +26285,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>1060</v>
@@ -26298,7 +26297,7 @@
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>1060</v>
@@ -26485,7 +26484,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1060</v>
@@ -26562,7 +26561,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>1060</v>
@@ -26600,9 +26599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="16" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26901,7 +26900,7 @@
         <v>222</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>324</v>
@@ -26945,7 +26944,7 @@
         <v>66</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>324</v>
@@ -27236,7 +27235,7 @@
         <v>24</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>324</v>
@@ -27399,7 +27398,7 @@
         <v>282</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>323</v>
@@ -27437,7 +27436,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>323</v>
@@ -27488,7 +27487,7 @@
         <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>323</v>
@@ -27510,7 +27509,7 @@
         <v>210</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1452</v>
@@ -27521,7 +27520,7 @@
         <v>196</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1452</v>
@@ -27532,7 +27531,7 @@
         <v>185</v>
       </c>
       <c r="B18" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>323</v>
@@ -27543,7 +27542,7 @@
         <v>270</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1452</v>
@@ -27593,7 +27592,7 @@
         <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>323</v>
@@ -27604,7 +27603,7 @@
         <v>159</v>
       </c>
       <c r="B25" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>323</v>
@@ -28022,7 +28021,7 @@
         <v>511</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1453</v>
@@ -28052,7 +28051,7 @@
         <v>250</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>321</v>
@@ -28074,7 +28073,7 @@
         <v>162</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1453</v>

</xml_diff>